<commit_message>
Ajuste formato de excel cargue diccionarios
</commit_message>
<xml_diff>
--- a/assets/formatos_cargue/32_formato_cargue_diccionarios.xlsx
+++ b/assets/formatos_cargue/32_formato_cargue_diccionarios.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t>bigbang.txt</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>n5-052</t>
   </si>
@@ -30,9 +27,6 @@
     <t>cod tema</t>
   </si>
   <si>
-    <t>archivo lectura</t>
-  </si>
-  <si>
     <t>palabra 1</t>
   </si>
   <si>
@@ -96,12 +90,6 @@
     <t>Big Bang</t>
   </si>
   <si>
-    <t>También llamada Gran Explosión</t>
-  </si>
-  <si>
-    <t>Densidad</t>
-  </si>
-  <si>
     <t>El término densidad proviene del campo de la física y la química, en los que específicamente alude a la relación que existe entre la masa de una sustancia (o de un cuerpo) y su volumen.</t>
   </si>
   <si>
@@ -109,6 +97,36 @@
   </si>
   <si>
     <t>El Big Bang</t>
+  </si>
+  <si>
+    <t>archivo imagen</t>
+  </si>
+  <si>
+    <t>imagen.jpg</t>
+  </si>
+  <si>
+    <t>También llamada Gran Explosión, por su traducción en inglés.</t>
+  </si>
+  <si>
+    <t>densidad</t>
+  </si>
+  <si>
+    <t>Stephen Hawking</t>
+  </si>
+  <si>
+    <t>Stephen William Hawking (Oxford, 8 de enero de 1942-Cambridge, 14 de marzo de 2018)​ fue un físico teórico, astrofísico, cosmólogo y divulgador científico británico.</t>
+  </si>
+  <si>
+    <t>singularidad</t>
+  </si>
+  <si>
+    <t>Una singularidad gravitacional o espaciotemporal, de modo informal y desde un punto de vista físico, puede definirse como una zona del espacio-tiempo donde no se puede definir alguna magnitud física relacionada con los campos gravitatorios, tales como la curvatura, u otras.</t>
+  </si>
+  <si>
+    <t>Einstein</t>
+  </si>
+  <si>
+    <t>Albert Einstein (Ulm, Imperio alemán, 14 de marzo de 1879-Princeton, Estados Unidos, 18 de abril de 1955) fue un físico alemán de origen judío, nacionalizado después suizo, austriaco y estadounidense. Se lo considera el científico más importante, conocido y popular del siglo XX.1</t>
   </si>
 </sst>
 </file>
@@ -503,7 +521,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,102 +536,131 @@
     <col min="9" max="9" width="40.7109375" style="4" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" style="4" customWidth="1"/>
     <col min="11" max="11" width="40.7109375" style="4" customWidth="1"/>
-    <col min="12" max="23" width="16.7109375" style="4" customWidth="1"/>
+    <col min="12" max="22" width="16.7109375" style="4" customWidth="1"/>
+    <col min="23" max="23" width="42" style="4" customWidth="1"/>
     <col min="24" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="F2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>27</v>
+      <c r="H2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>